<commit_message>
Improve score card exporting
</commit_message>
<xml_diff>
--- a/public/static/score-card.xlsx
+++ b/public/static/score-card.xlsx
@@ -543,9 +543,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -584,6 +581,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2489,7 +2489,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -2534,14 +2534,14 @@
       <c r="D2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="31" t="s">
+      <c r="E2" s="36"/>
+      <c r="F2" s="30" t="s">
         <v>22</v>
       </c>
       <c r="G2" s="40"/>
       <c r="H2" s="41"/>
       <c r="I2" s="42"/>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="35" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="4"/>
@@ -2579,7 +2579,7 @@
       <c r="I3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="31" t="s">
         <v>17</v>
       </c>
       <c r="K3" s="4"/>
@@ -2599,16 +2599,16 @@
       <c r="C4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="23" t="s">
         <v>7</v>
       </c>
       <c r="H4" s="6" t="s">
@@ -2617,7 +2617,7 @@
       <c r="I4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="33" t="s">
+      <c r="J4" s="32" t="s">
         <v>16</v>
       </c>
       <c r="K4" s="4"/>
@@ -2635,7 +2635,7 @@
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="27"/>
+      <c r="H5" s="26"/>
       <c r="I5" s="15"/>
       <c r="J5" s="14"/>
       <c r="K5" s="4"/>
@@ -2655,7 +2655,7 @@
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
-      <c r="H6" s="28"/>
+      <c r="H6" s="27"/>
       <c r="I6" s="15"/>
       <c r="J6" s="14"/>
       <c r="K6" s="4"/>
@@ -2675,7 +2675,7 @@
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="29"/>
+      <c r="H7" s="28"/>
       <c r="I7" s="15"/>
       <c r="J7" s="14"/>
       <c r="K7" s="4"/>
@@ -2695,7 +2695,7 @@
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
-      <c r="H8" s="28"/>
+      <c r="H8" s="27"/>
       <c r="I8" s="15"/>
       <c r="J8" s="14"/>
       <c r="K8" s="4"/>
@@ -2715,7 +2715,7 @@
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
-      <c r="H9" s="30"/>
+      <c r="H9" s="29"/>
       <c r="I9" s="15"/>
       <c r="J9" s="14"/>
       <c r="K9" s="4"/>
@@ -2726,18 +2726,18 @@
       <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16" s="21" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="34"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="33"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -2774,14 +2774,14 @@
       <c r="D13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="23"/>
-      <c r="F13" s="31" t="s">
+      <c r="E13" s="36"/>
+      <c r="F13" s="30" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="40"/>
       <c r="H13" s="41"/>
       <c r="I13" s="42"/>
-      <c r="J13" s="36" t="s">
+      <c r="J13" s="35" t="s">
         <v>25</v>
       </c>
       <c r="K13" s="4"/>
@@ -2819,7 +2819,7 @@
       <c r="I14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="32" t="s">
+      <c r="J14" s="31" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="4"/>
@@ -2839,16 +2839,16 @@
       <c r="C15" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="23" t="s">
         <v>7</v>
       </c>
       <c r="H15" s="6" t="s">
@@ -2857,7 +2857,7 @@
       <c r="I15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="33" t="s">
+      <c r="J15" s="32" t="s">
         <v>16</v>
       </c>
       <c r="K15" s="4"/>
@@ -2875,7 +2875,7 @@
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
-      <c r="H16" s="27"/>
+      <c r="H16" s="26"/>
       <c r="I16" s="15"/>
       <c r="J16" s="14"/>
       <c r="K16" s="4"/>
@@ -2895,7 +2895,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
-      <c r="H17" s="28"/>
+      <c r="H17" s="27"/>
       <c r="I17" s="15"/>
       <c r="J17" s="14"/>
       <c r="K17" s="4"/>
@@ -2915,7 +2915,7 @@
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
-      <c r="H18" s="29"/>
+      <c r="H18" s="28"/>
       <c r="I18" s="15"/>
       <c r="J18" s="14"/>
       <c r="K18" s="4"/>
@@ -2935,7 +2935,7 @@
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
-      <c r="H19" s="28"/>
+      <c r="H19" s="27"/>
       <c r="I19" s="15"/>
       <c r="J19" s="14"/>
       <c r="K19" s="4"/>
@@ -2955,7 +2955,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
-      <c r="H20" s="30"/>
+      <c r="H20" s="29"/>
       <c r="I20" s="15"/>
       <c r="J20" s="14"/>
       <c r="K20" s="4"/>
@@ -2966,18 +2966,18 @@
       <c r="P20" s="4"/>
     </row>
     <row r="21" spans="1:16" s="21" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="34"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="33"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
@@ -3014,14 +3014,14 @@
       <c r="D24" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="23"/>
-      <c r="F24" s="31" t="s">
+      <c r="E24" s="36"/>
+      <c r="F24" s="30" t="s">
         <v>22</v>
       </c>
       <c r="G24" s="40"/>
       <c r="H24" s="41"/>
       <c r="I24" s="42"/>
-      <c r="J24" s="36" t="s">
+      <c r="J24" s="35" t="s">
         <v>25</v>
       </c>
       <c r="K24" s="4"/>
@@ -3059,7 +3059,7 @@
       <c r="I25" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="32" t="s">
+      <c r="J25" s="31" t="s">
         <v>17</v>
       </c>
       <c r="K25" s="4"/>
@@ -3079,16 +3079,16 @@
       <c r="C26" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F26" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="24" t="s">
+      <c r="G26" s="23" t="s">
         <v>7</v>
       </c>
       <c r="H26" s="6" t="s">
@@ -3097,7 +3097,7 @@
       <c r="I26" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J26" s="33" t="s">
+      <c r="J26" s="32" t="s">
         <v>16</v>
       </c>
       <c r="K26" s="4"/>
@@ -3115,7 +3115,7 @@
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
-      <c r="H27" s="27"/>
+      <c r="H27" s="26"/>
       <c r="I27" s="15"/>
       <c r="J27" s="14"/>
       <c r="K27" s="4"/>
@@ -3135,7 +3135,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
-      <c r="H28" s="28"/>
+      <c r="H28" s="27"/>
       <c r="I28" s="15"/>
       <c r="J28" s="14"/>
       <c r="K28" s="4"/>
@@ -3155,7 +3155,7 @@
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
-      <c r="H29" s="29"/>
+      <c r="H29" s="28"/>
       <c r="I29" s="15"/>
       <c r="J29" s="14"/>
       <c r="K29" s="4"/>
@@ -3175,7 +3175,7 @@
       <c r="E30" s="16"/>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
-      <c r="H30" s="28"/>
+      <c r="H30" s="27"/>
       <c r="I30" s="15"/>
       <c r="J30" s="14"/>
       <c r="K30" s="4"/>
@@ -3195,7 +3195,7 @@
       <c r="E31" s="16"/>
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
-      <c r="H31" s="30"/>
+      <c r="H31" s="29"/>
       <c r="I31" s="15"/>
       <c r="J31" s="14"/>
       <c r="K31" s="4"/>
@@ -3206,18 +3206,18 @@
       <c r="P31" s="4"/>
     </row>
     <row r="32" spans="1:16" s="21" customFormat="1" ht="15.75" thickTop="1">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="34"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="33"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>

</xml_diff>